<commit_message>
fix: replace broken MSDS URL
</commit_message>
<xml_diff>
--- a/Soap_blend.xlsx
+++ b/Soap_blend.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Downloads\hand_soap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Dropbox\Recipes\hand_soap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8BBFB8-EC24-4C1A-8C0F-8FEAE92C9E1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B070543-0642-4CCA-B03C-9B013F0EA0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{B92A62B0-C284-4325-A6E4-B9DC043911A6}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$7</definedName>
     <definedName name="Volume">Sheet1!$K$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -26,6 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -984,7 +986,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G7"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,8 +999,7 @@
     <col min="6" max="7" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: increase oil to 6 g
Original proportion led to dry hands.
</commit_message>
<xml_diff>
--- a/Soap_blend.xlsx
+++ b/Soap_blend.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Dropbox\Recipes\hand_soap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\GitHub\hand_soap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B070543-0642-4CCA-B03C-9B013F0EA0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D148E930-8C27-42F5-8B39-25BECD76B098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{B92A62B0-C284-4325-A6E4-B9DC043911A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B92A62B0-C284-4325-A6E4-B9DC043911A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -251,7 +245,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
@@ -291,6 +285,7 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -299,9 +294,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -336,15 +328,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -394,13 +377,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -436,6 +427,65 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -484,39 +534,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -534,28 +551,11 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -567,17 +567,12 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -652,21 +647,21 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1668803E-B398-438E-B3DE-BA9EC7EA9607}" name="Ingredients" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{052818CF-781A-4A4E-B42F-D2AD16722113}" name="Raw Amt" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="1" xr3:uid="{1668803E-B398-438E-B3DE-BA9EC7EA9607}" name="Ingredients" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{052818CF-781A-4A4E-B42F-D2AD16722113}" name="Raw Amt" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="5">
       <totalsRowFormula>CONVERT(Blend[[#Totals],[Amount]],D7,C2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{16174C3D-3388-45C7-84D3-DC51F1C1F1B2}" name="Raw Units" totalsRowLabel="oz" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{2F746F7C-9121-4E45-8D84-A0FA9A98967D}" name="Amount" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="3" xr3:uid="{16174C3D-3388-45C7-84D3-DC51F1C1F1B2}" name="Raw Units" totalsRowLabel="oz" dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{2F746F7C-9121-4E45-8D84-A0FA9A98967D}" name="Amount" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="3">
       <calculatedColumnFormula>CONVERT(Blend[[#This Row],[Raw Amt]],Blend[[#This Row],[Raw Units]],D$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E2D46B65-DF29-447C-B18F-7D67FD8448E0}" name="Scaled Vol" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5">
+    <tableColumn id="4" xr3:uid="{E2D46B65-DF29-447C-B18F-7D67FD8448E0}" name="Scaled Vol" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="2">
       <calculatedColumnFormula>Volume/Blend[[#Totals],[Amount]]*Blend[[#This Row],[Amount]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7C86046F-C060-49F1-85DD-63FCAD6001AB}" name="Density" dataDxfId="4" totalsRowDxfId="3">
+    <tableColumn id="8" xr3:uid="{7C86046F-C060-49F1-85DD-63FCAD6001AB}" name="Density" dataDxfId="8" totalsRowDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Blend[[#This Row],[Ingredients]],Ingredients[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A2890646-39D0-4A24-B95C-E22BFC304F60}" name="Scaled Mass" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1">
+    <tableColumn id="7" xr3:uid="{A2890646-39D0-4A24-B95C-E22BFC304F60}" name="Scaled Mass" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="0">
       <calculatedColumnFormula>Blend[[#This Row],[Scaled Vol]]*Blend[[#This Row],[Density]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -675,7 +670,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{205B2791-4AAE-4298-9B77-7D4A8AE6CE11}" name="Ingredients" displayName="Ingredients" ref="N1:P6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{205B2791-4AAE-4298-9B77-7D4A8AE6CE11}" name="Ingredients" displayName="Ingredients" ref="N1:P6" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="N1:P6" xr:uid="{8869B219-6989-4315-BB33-5A758269B9CD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1E0718B6-8EDA-404B-80AC-B594EC6B96F1}" name="Name"/>
@@ -986,7 +981,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1042,18 +1037,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="24">
-        <v>10.666666666666666</v>
+        <v>10.464957199674283</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="5">
         <f>CONVERT(Blend[[#This Row],[Raw Amt]],Blend[[#This Row],[Raw Units]],D$7)</f>
-        <v>315.45098200000001</v>
+        <v>309.48572111486459</v>
       </c>
       <c r="E2" s="9">
         <f>Volume/Blend[[#Totals],[Amount]]*Blend[[#This Row],[Amount]]</f>
-        <v>184.01307283333335</v>
+        <v>180.53333731700428</v>
       </c>
       <c r="F2" s="8">
         <f>VLOOKUP(Blend[[#This Row],[Ingredients]],Ingredients[],3,FALSE)</f>
@@ -1061,7 +1056,7 @@
       </c>
       <c r="G2" s="9">
         <f>Blend[[#This Row],[Scaled Vol]]*Blend[[#This Row],[Density]]</f>
-        <v>184.01307283333335</v>
+        <v>180.53333731700428</v>
       </c>
       <c r="I2" s="16">
         <v>7</v>
@@ -1090,7 +1085,7 @@
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="24">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -1102,7 +1097,7 @@
       </c>
       <c r="E3" s="9">
         <f>Volume/Blend[[#Totals],[Amount]]*Blend[[#This Row],[Amount]]</f>
-        <v>17.251225578125002</v>
+        <v>17.251225578124995</v>
       </c>
       <c r="F3" s="8">
         <f>VLOOKUP(Blend[[#This Row],[Ingredients]],Ingredients[],3,FALSE)</f>
@@ -1110,7 +1105,7 @@
       </c>
       <c r="G3" s="9">
         <f>Blend[[#This Row],[Scaled Vol]]*Blend[[#This Row],[Density]]</f>
-        <v>17.423737833906252</v>
+        <v>17.423737833906245</v>
       </c>
       <c r="K3" s="1"/>
       <c r="N3" t="s">
@@ -1127,19 +1122,19 @@
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="7">
-        <v>1</v>
+      <c r="B4" s="24">
+        <v>2.2102568019543289</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="5">
         <f>CONVERT(Blend[[#This Row],[Raw Amt]],Blend[[#This Row],[Raw Units]],D$7)</f>
-        <v>4.9289215937500002</v>
+        <v>10.894182478885508</v>
       </c>
       <c r="E4" s="9">
         <f>Volume/Blend[[#Totals],[Amount]]*Blend[[#This Row],[Amount]]</f>
-        <v>2.8752042630208337</v>
+        <v>6.3549397793498779</v>
       </c>
       <c r="F4" s="8">
         <f>VLOOKUP(Blend[[#This Row],[Ingredients]],Ingredients[],3,FALSE)</f>
@@ -1147,7 +1142,7 @@
       </c>
       <c r="G4" s="9">
         <f>Blend[[#This Row],[Scaled Vol]]*Blend[[#This Row],[Density]]</f>
-        <v>2.7601960925000002</v>
+        <v>6.1007421881758823</v>
       </c>
       <c r="K4" s="1"/>
       <c r="N4" t="s">
@@ -1164,7 +1159,7 @@
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="25">
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1176,7 +1171,7 @@
       </c>
       <c r="E5" s="9">
         <f>Volume/Blend[[#Totals],[Amount]]*Blend[[#This Row],[Amount]]</f>
-        <v>2.8752042630208337</v>
+        <v>2.8752042630208323</v>
       </c>
       <c r="F5" s="8">
         <f>VLOOKUP(Blend[[#This Row],[Ingredients]],Ingredients[],3,FALSE)</f>
@@ -1184,7 +1179,7 @@
       </c>
       <c r="G5" s="9">
         <f>Blend[[#This Row],[Scaled Vol]]*Blend[[#This Row],[Density]]</f>
-        <v>3.5940053287760421</v>
+        <v>3.5940053287760403</v>
       </c>
       <c r="K5" s="1"/>
       <c r="N5" t="s">
@@ -1203,23 +1198,23 @@
       </c>
       <c r="B6" s="23">
         <f>CONVERT(Blend[[#Totals],[Amount]],D7,C2)</f>
-        <v>12</v>
+        <v>12.000000000000004</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="11">
         <f>SUBTOTAL(109,Blend[Amount])</f>
-        <v>354.88235474999999</v>
+        <v>354.8823547500001</v>
       </c>
       <c r="E6" s="11">
         <f>SUBTOTAL(109,Blend[Scaled Vol])</f>
-        <v>207.01470693750002</v>
+        <v>207.01470693749999</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11">
         <f>SUBTOTAL(109,Blend[Scaled Mass])</f>
-        <v>207.79101208851563</v>
+        <v>207.65182266786243</v>
       </c>
       <c r="N6" t="s">
         <v>1</v>

</xml_diff>